<commit_message>
finished Women award data
</commit_message>
<xml_diff>
--- a/Awards/Women/Cross Country.xlsx
+++ b/Awards/Women/Cross Country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dengjiahao\Desktop\Athlete\Awards\Women\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864AA325-D62F-4B43-9375-0B6D4CA25598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C39441-9146-4AF4-83FE-5CAD5A8533BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="1710" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="65">
   <si>
     <t>Year</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>Paige Wheeler</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Midwest Conference</t>
   </si>
 </sst>
 </file>
@@ -533,19 +545,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,8 +568,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2007</v>
       </c>
@@ -566,8 +582,11 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2006</v>
       </c>
@@ -577,8 +596,11 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2021</v>
       </c>
@@ -588,8 +610,11 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2012</v>
       </c>
@@ -599,8 +624,11 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2013</v>
       </c>
@@ -610,8 +638,11 @@
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2011</v>
       </c>
@@ -621,8 +652,11 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
@@ -632,8 +666,11 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2006</v>
       </c>
@@ -643,8 +680,11 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2006</v>
       </c>
@@ -654,8 +694,11 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2006</v>
       </c>
@@ -665,8 +708,11 @@
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2006</v>
       </c>
@@ -676,8 +722,11 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2006</v>
       </c>
@@ -687,8 +736,11 @@
       <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2006</v>
       </c>
@@ -698,8 +750,11 @@
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2006</v>
       </c>
@@ -709,8 +764,11 @@
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2006</v>
       </c>
@@ -720,8 +778,11 @@
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2012</v>
       </c>
@@ -731,8 +792,11 @@
       <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -742,8 +806,11 @@
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -753,8 +820,11 @@
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -764,8 +834,11 @@
       <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2022</v>
       </c>
@@ -775,8 +848,11 @@
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2021</v>
       </c>
@@ -786,8 +862,11 @@
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2019</v>
       </c>
@@ -797,8 +876,11 @@
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2018</v>
       </c>
@@ -808,8 +890,11 @@
       <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2016</v>
       </c>
@@ -819,8 +904,11 @@
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2015</v>
       </c>
@@ -830,8 +918,11 @@
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2015</v>
       </c>
@@ -841,8 +932,11 @@
       <c r="C27" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2014</v>
       </c>
@@ -852,8 +946,11 @@
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2014</v>
       </c>
@@ -863,8 +960,11 @@
       <c r="C29" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2013</v>
       </c>
@@ -874,8 +974,11 @@
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2013</v>
       </c>
@@ -885,8 +988,11 @@
       <c r="C31" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2012</v>
       </c>
@@ -896,8 +1002,11 @@
       <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2007</v>
       </c>
@@ -907,8 +1016,11 @@
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2007</v>
       </c>
@@ -918,8 +1030,11 @@
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2007</v>
       </c>
@@ -929,8 +1044,11 @@
       <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2006</v>
       </c>
@@ -940,8 +1058,11 @@
       <c r="C36" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2006</v>
       </c>
@@ -951,8 +1072,11 @@
       <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2006</v>
       </c>
@@ -962,8 +1086,11 @@
       <c r="C38" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2006</v>
       </c>
@@ -973,8 +1100,11 @@
       <c r="C39" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2006</v>
       </c>
@@ -984,8 +1114,11 @@
       <c r="C40" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2006</v>
       </c>
@@ -995,8 +1128,11 @@
       <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2024</v>
       </c>
@@ -1006,8 +1142,11 @@
       <c r="C42" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -1017,8 +1156,11 @@
       <c r="C43" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2021</v>
       </c>
@@ -1028,8 +1170,11 @@
       <c r="C44" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2019</v>
       </c>
@@ -1039,8 +1184,11 @@
       <c r="C45" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2018</v>
       </c>
@@ -1050,8 +1198,11 @@
       <c r="C46" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2017</v>
       </c>
@@ -1061,8 +1212,11 @@
       <c r="C47" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
@@ -1072,8 +1226,11 @@
       <c r="C48" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2016</v>
       </c>
@@ -1083,8 +1240,11 @@
       <c r="C49" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2015</v>
       </c>
@@ -1094,8 +1254,11 @@
       <c r="C50" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2014</v>
       </c>
@@ -1105,8 +1268,11 @@
       <c r="C51" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2013</v>
       </c>
@@ -1116,8 +1282,11 @@
       <c r="C52" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2013</v>
       </c>
@@ -1127,8 +1296,11 @@
       <c r="C53" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2012</v>
       </c>
@@ -1138,8 +1310,11 @@
       <c r="C54" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2012</v>
       </c>
@@ -1149,8 +1324,11 @@
       <c r="C55" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2011</v>
       </c>
@@ -1160,8 +1338,11 @@
       <c r="C56" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2007</v>
       </c>
@@ -1171,8 +1352,11 @@
       <c r="C57" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2007</v>
       </c>
@@ -1182,8 +1366,11 @@
       <c r="C58" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2007</v>
       </c>
@@ -1193,8 +1380,11 @@
       <c r="C59" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2006</v>
       </c>
@@ -1204,8 +1394,11 @@
       <c r="C60" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2006</v>
       </c>
@@ -1215,8 +1408,11 @@
       <c r="C61" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2006</v>
       </c>
@@ -1226,8 +1422,11 @@
       <c r="C62" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2006</v>
       </c>
@@ -1237,8 +1436,11 @@
       <c r="C63" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2006</v>
       </c>
@@ -1248,8 +1450,11 @@
       <c r="C64" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2006</v>
       </c>
@@ -1259,8 +1464,11 @@
       <c r="C65" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2004</v>
       </c>
@@ -1270,8 +1478,11 @@
       <c r="C66" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2003</v>
       </c>
@@ -1281,8 +1492,11 @@
       <c r="C67" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2006</v>
       </c>
@@ -1292,8 +1506,11 @@
       <c r="C68" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2024</v>
       </c>
@@ -1303,8 +1520,11 @@
       <c r="C69" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2024</v>
       </c>
@@ -1314,8 +1534,11 @@
       <c r="C70" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
@@ -1325,8 +1548,11 @@
       <c r="C71" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -1336,8 +1562,11 @@
       <c r="C72" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -1347,8 +1576,11 @@
       <c r="C73" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2013</v>
       </c>
@@ -1358,8 +1590,11 @@
       <c r="C74" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>2012</v>
       </c>
@@ -1369,8 +1604,11 @@
       <c r="C75" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>2007</v>
       </c>
@@ -1380,8 +1618,11 @@
       <c r="C76" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>2006</v>
       </c>
@@ -1391,8 +1632,11 @@
       <c r="C77" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>2022</v>
       </c>
@@ -1402,8 +1646,11 @@
       <c r="C78" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>2022</v>
       </c>
@@ -1413,8 +1660,11 @@
       <c r="C79" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>2019</v>
       </c>
@@ -1424,8 +1674,11 @@
       <c r="C80" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>2014</v>
       </c>
@@ -1435,8 +1688,11 @@
       <c r="C81" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>2013</v>
       </c>
@@ -1446,8 +1702,11 @@
       <c r="C82" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>2011</v>
       </c>
@@ -1457,8 +1716,11 @@
       <c r="C83" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>2009</v>
       </c>
@@ -1468,8 +1730,11 @@
       <c r="C84" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>2006</v>
       </c>
@@ -1479,8 +1744,11 @@
       <c r="C85" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>2005</v>
       </c>
@@ -1490,8 +1758,11 @@
       <c r="C86" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>2004</v>
       </c>
@@ -1501,8 +1772,11 @@
       <c r="C87" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>2024</v>
       </c>
@@ -1512,8 +1786,11 @@
       <c r="C88" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>2024</v>
       </c>
@@ -1523,8 +1800,11 @@
       <c r="C89" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>2024</v>
       </c>
@@ -1534,8 +1814,11 @@
       <c r="C90" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>2024</v>
       </c>
@@ -1545,8 +1828,11 @@
       <c r="C91" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>2024</v>
       </c>
@@ -1556,8 +1842,11 @@
       <c r="C92" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>2024</v>
       </c>
@@ -1567,8 +1856,11 @@
       <c r="C93" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>2024</v>
       </c>
@@ -1578,8 +1870,11 @@
       <c r="C94" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>2023</v>
       </c>
@@ -1589,8 +1884,11 @@
       <c r="C95" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>2023</v>
       </c>
@@ -1600,8 +1898,11 @@
       <c r="C96" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>2023</v>
       </c>
@@ -1611,8 +1912,11 @@
       <c r="C97" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>2023</v>
       </c>
@@ -1622,8 +1926,11 @@
       <c r="C98" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>2023</v>
       </c>
@@ -1633,8 +1940,11 @@
       <c r="C99" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>2022</v>
       </c>
@@ -1644,8 +1954,11 @@
       <c r="C100" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>2022</v>
       </c>
@@ -1655,8 +1968,11 @@
       <c r="C101" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>2022</v>
       </c>
@@ -1666,8 +1982,11 @@
       <c r="C102" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>2022</v>
       </c>
@@ -1677,8 +1996,11 @@
       <c r="C103" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>2022</v>
       </c>
@@ -1688,8 +2010,11 @@
       <c r="C104" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>2022</v>
       </c>
@@ -1699,8 +2024,11 @@
       <c r="C105" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>2022</v>
       </c>
@@ -1710,8 +2038,11 @@
       <c r="C106" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>2022</v>
       </c>
@@ -1721,8 +2052,11 @@
       <c r="C107" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>2021</v>
       </c>
@@ -1732,8 +2066,11 @@
       <c r="C108" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>2021</v>
       </c>
@@ -1743,8 +2080,11 @@
       <c r="C109" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>2021</v>
       </c>
@@ -1754,8 +2094,11 @@
       <c r="C110" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>2021</v>
       </c>
@@ -1765,8 +2108,11 @@
       <c r="C111" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>2019</v>
       </c>
@@ -1776,8 +2122,11 @@
       <c r="C112" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>2019</v>
       </c>
@@ -1787,8 +2136,11 @@
       <c r="C113" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>2019</v>
       </c>
@@ -1798,8 +2150,11 @@
       <c r="C114" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>2019</v>
       </c>
@@ -1809,8 +2164,11 @@
       <c r="C115" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>2019</v>
       </c>
@@ -1820,8 +2178,11 @@
       <c r="C116" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>2018</v>
       </c>
@@ -1831,8 +2192,11 @@
       <c r="C117" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>2018</v>
       </c>
@@ -1842,8 +2206,11 @@
       <c r="C118" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>2018</v>
       </c>
@@ -1853,8 +2220,11 @@
       <c r="C119" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>2017</v>
       </c>
@@ -1864,8 +2234,11 @@
       <c r="C120" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>2017</v>
       </c>
@@ -1875,8 +2248,11 @@
       <c r="C121" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>2017</v>
       </c>
@@ -1886,8 +2262,11 @@
       <c r="C122" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>2016</v>
       </c>
@@ -1897,8 +2276,11 @@
       <c r="C123" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>2016</v>
       </c>
@@ -1908,8 +2290,11 @@
       <c r="C124" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>2016</v>
       </c>
@@ -1919,8 +2304,11 @@
       <c r="C125" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>2016</v>
       </c>
@@ -1930,8 +2318,11 @@
       <c r="C126" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>2015</v>
       </c>
@@ -1941,8 +2332,11 @@
       <c r="C127" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>2015</v>
       </c>
@@ -1952,8 +2346,11 @@
       <c r="C128" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>2015</v>
       </c>
@@ -1963,8 +2360,11 @@
       <c r="C129" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>2014</v>
       </c>
@@ -1974,8 +2374,11 @@
       <c r="C130" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>2014</v>
       </c>
@@ -1985,8 +2388,11 @@
       <c r="C131" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>2014</v>
       </c>
@@ -1996,8 +2402,11 @@
       <c r="C132" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>2014</v>
       </c>
@@ -2007,8 +2416,11 @@
       <c r="C133" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>2014</v>
       </c>
@@ -2018,8 +2430,11 @@
       <c r="C134" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>2013</v>
       </c>
@@ -2029,8 +2444,11 @@
       <c r="C135" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>2013</v>
       </c>
@@ -2040,8 +2458,11 @@
       <c r="C136" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>2013</v>
       </c>
@@ -2051,8 +2472,11 @@
       <c r="C137" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>2013</v>
       </c>
@@ -2062,8 +2486,11 @@
       <c r="C138" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>2012</v>
       </c>
@@ -2073,8 +2500,11 @@
       <c r="C139" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>2012</v>
       </c>
@@ -2084,8 +2514,11 @@
       <c r="C140" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>2012</v>
       </c>
@@ -2095,8 +2528,11 @@
       <c r="C141" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>2011</v>
       </c>
@@ -2106,8 +2542,11 @@
       <c r="C142" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>2011</v>
       </c>
@@ -2117,8 +2556,11 @@
       <c r="C143" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>2011</v>
       </c>
@@ -2128,8 +2570,11 @@
       <c r="C144" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>2011</v>
       </c>
@@ -2139,8 +2584,11 @@
       <c r="C145" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>2011</v>
       </c>
@@ -2150,8 +2598,11 @@
       <c r="C146" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>2010</v>
       </c>
@@ -2161,8 +2612,11 @@
       <c r="C147" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>2010</v>
       </c>
@@ -2172,8 +2626,11 @@
       <c r="C148" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>2010</v>
       </c>
@@ -2183,8 +2640,11 @@
       <c r="C149" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>2009</v>
       </c>
@@ -2194,8 +2654,11 @@
       <c r="C150" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>2009</v>
       </c>
@@ -2205,8 +2668,11 @@
       <c r="C151" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>2009</v>
       </c>
@@ -2216,8 +2682,11 @@
       <c r="C152" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>2009</v>
       </c>
@@ -2227,8 +2696,11 @@
       <c r="C153" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>2008</v>
       </c>
@@ -2238,8 +2710,11 @@
       <c r="C154" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>2008</v>
       </c>
@@ -2249,8 +2724,11 @@
       <c r="C155" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>2008</v>
       </c>
@@ -2260,8 +2738,11 @@
       <c r="C156" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>2008</v>
       </c>
@@ -2271,8 +2752,11 @@
       <c r="C157" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>2007</v>
       </c>
@@ -2282,8 +2766,11 @@
       <c r="C158" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>2007</v>
       </c>
@@ -2293,8 +2780,11 @@
       <c r="C159" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>2007</v>
       </c>
@@ -2304,8 +2794,11 @@
       <c r="C160" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>2007</v>
       </c>
@@ -2315,8 +2808,11 @@
       <c r="C161" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>2007</v>
       </c>
@@ -2326,8 +2822,11 @@
       <c r="C162" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>2006</v>
       </c>
@@ -2337,8 +2836,11 @@
       <c r="C163" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>2006</v>
       </c>
@@ -2348,8 +2850,11 @@
       <c r="C164" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>2006</v>
       </c>
@@ -2359,8 +2864,11 @@
       <c r="C165" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>2006</v>
       </c>
@@ -2370,8 +2878,11 @@
       <c r="C166" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>2006</v>
       </c>
@@ -2381,8 +2892,11 @@
       <c r="C167" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>2006</v>
       </c>
@@ -2392,8 +2906,11 @@
       <c r="C168" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>2006</v>
       </c>
@@ -2403,8 +2920,11 @@
       <c r="C169" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>2006</v>
       </c>
@@ -2414,8 +2934,11 @@
       <c r="C170" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>2006</v>
       </c>
@@ -2425,8 +2948,11 @@
       <c r="C171" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>2005</v>
       </c>
@@ -2436,8 +2962,11 @@
       <c r="C172" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>2005</v>
       </c>
@@ -2447,8 +2976,11 @@
       <c r="C173" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>2005</v>
       </c>
@@ -2458,8 +2990,11 @@
       <c r="C174" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>2005</v>
       </c>
@@ -2469,8 +3004,11 @@
       <c r="C175" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>2005</v>
       </c>
@@ -2480,8 +3018,11 @@
       <c r="C176" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>2005</v>
       </c>
@@ -2491,8 +3032,11 @@
       <c r="C177" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>2004</v>
       </c>
@@ -2502,8 +3046,11 @@
       <c r="C178" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>2004</v>
       </c>
@@ -2513,8 +3060,11 @@
       <c r="C179" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>2004</v>
       </c>
@@ -2524,8 +3074,11 @@
       <c r="C180" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>2004</v>
       </c>
@@ -2535,8 +3088,11 @@
       <c r="C181" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>2004</v>
       </c>
@@ -2546,8 +3102,11 @@
       <c r="C182" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>2004</v>
       </c>
@@ -2557,8 +3116,11 @@
       <c r="C183" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>2003</v>
       </c>
@@ -2568,8 +3130,11 @@
       <c r="C184" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>2003</v>
       </c>
@@ -2579,8 +3144,11 @@
       <c r="C185" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>2003</v>
       </c>
@@ -2589,6 +3157,9 @@
       </c>
       <c r="C186" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="D186" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some awards data
</commit_message>
<xml_diff>
--- a/Awards/Women/Cross Country.xlsx
+++ b/Awards/Women/Cross Country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dengjiahao\Desktop\Athlete\Awards\Women\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C39441-9146-4AF4-83FE-5CAD5A8533BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFECCD61-29FC-4638-B1D6-15912C6A054A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="15090" windowHeight="9130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>Coach of the Year</t>
   </si>
   <si>
-    <t>CoSIDA Academic All-District (first team)</t>
-  </si>
-  <si>
     <t>Mira Diamond-Berman</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Midwest Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoSIDA Academic All-District </t>
   </si>
 </sst>
 </file>
@@ -547,18 +547,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,10 +569,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2007</v>
       </c>
@@ -583,10 +583,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2006</v>
       </c>
@@ -597,10 +597,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2021</v>
       </c>
@@ -611,10 +611,10 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2012</v>
       </c>
@@ -625,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2013</v>
       </c>
@@ -639,10 +639,10 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2011</v>
       </c>
@@ -653,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
@@ -667,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2006</v>
       </c>
@@ -681,10 +681,10 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2006</v>
       </c>
@@ -695,10 +695,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2006</v>
       </c>
@@ -709,10 +709,10 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2006</v>
       </c>
@@ -723,10 +723,10 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2006</v>
       </c>
@@ -737,10 +737,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2006</v>
       </c>
@@ -751,10 +751,10 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2006</v>
       </c>
@@ -765,10 +765,10 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2006</v>
       </c>
@@ -779,10 +779,10 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2012</v>
       </c>
@@ -793,10 +793,10 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2023</v>
       </c>
@@ -807,10 +807,10 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2023</v>
       </c>
@@ -821,10 +821,10 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2023</v>
       </c>
@@ -835,10 +835,10 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2022</v>
       </c>
@@ -849,10 +849,10 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2021</v>
       </c>
@@ -863,10 +863,10 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2019</v>
       </c>
@@ -877,10 +877,10 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2018</v>
       </c>
@@ -891,10 +891,10 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2016</v>
       </c>
@@ -905,10 +905,10 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2015</v>
       </c>
@@ -919,10 +919,10 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2015</v>
       </c>
@@ -933,10 +933,10 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2014</v>
       </c>
@@ -947,10 +947,10 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2014</v>
       </c>
@@ -961,10 +961,10 @@
         <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2013</v>
       </c>
@@ -975,10 +975,10 @@
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2013</v>
       </c>
@@ -989,10 +989,10 @@
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>2012</v>
       </c>
@@ -1003,10 +1003,10 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>2007</v>
       </c>
@@ -1017,10 +1017,10 @@
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>2007</v>
       </c>
@@ -1031,10 +1031,10 @@
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>2007</v>
       </c>
@@ -1045,10 +1045,10 @@
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>2006</v>
       </c>
@@ -1059,10 +1059,10 @@
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>2006</v>
       </c>
@@ -1073,10 +1073,10 @@
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>2006</v>
       </c>
@@ -1087,10 +1087,10 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>2006</v>
       </c>
@@ -1101,10 +1101,10 @@
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>2006</v>
       </c>
@@ -1115,10 +1115,10 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>2006</v>
       </c>
@@ -1129,10 +1129,10 @@
         <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2024</v>
       </c>
@@ -1143,10 +1143,10 @@
         <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>2023</v>
       </c>
@@ -1157,10 +1157,10 @@
         <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>2021</v>
       </c>
@@ -1171,10 +1171,10 @@
         <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>2019</v>
       </c>
@@ -1185,10 +1185,10 @@
         <v>25</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2018</v>
       </c>
@@ -1199,10 +1199,10 @@
         <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>2017</v>
       </c>
@@ -1213,10 +1213,10 @@
         <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
@@ -1227,10 +1227,10 @@
         <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>2016</v>
       </c>
@@ -1241,10 +1241,10 @@
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>2015</v>
       </c>
@@ -1255,10 +1255,10 @@
         <v>25</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>2014</v>
       </c>
@@ -1269,10 +1269,10 @@
         <v>25</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>2013</v>
       </c>
@@ -1283,10 +1283,10 @@
         <v>25</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>2013</v>
       </c>
@@ -1297,10 +1297,10 @@
         <v>25</v>
       </c>
       <c r="D53" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>2012</v>
       </c>
@@ -1311,10 +1311,10 @@
         <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>2012</v>
       </c>
@@ -1325,10 +1325,10 @@
         <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>2011</v>
       </c>
@@ -1339,10 +1339,10 @@
         <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>2007</v>
       </c>
@@ -1353,10 +1353,10 @@
         <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2007</v>
       </c>
@@ -1367,10 +1367,10 @@
         <v>25</v>
       </c>
       <c r="D58" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2007</v>
       </c>
@@ -1381,10 +1381,10 @@
         <v>25</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>2006</v>
       </c>
@@ -1395,10 +1395,10 @@
         <v>25</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>2006</v>
       </c>
@@ -1409,10 +1409,10 @@
         <v>25</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2006</v>
       </c>
@@ -1423,10 +1423,10 @@
         <v>25</v>
       </c>
       <c r="D62" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>2006</v>
       </c>
@@ -1437,10 +1437,10 @@
         <v>25</v>
       </c>
       <c r="D63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>2006</v>
       </c>
@@ -1451,10 +1451,10 @@
         <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>2006</v>
       </c>
@@ -1465,10 +1465,10 @@
         <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>2004</v>
       </c>
@@ -1479,10 +1479,10 @@
         <v>25</v>
       </c>
       <c r="D66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>2003</v>
       </c>
@@ -1493,10 +1493,10 @@
         <v>25</v>
       </c>
       <c r="D67" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>2006</v>
       </c>
@@ -1507,10 +1507,10 @@
         <v>28</v>
       </c>
       <c r="D68" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>2024</v>
       </c>
@@ -1518,13 +1518,13 @@
         <v>17</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D69" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>2024</v>
       </c>
@@ -1532,27 +1532,27 @@
         <v>15</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D70" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>2023</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D71" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>2023</v>
       </c>
@@ -1560,13 +1560,13 @@
         <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D72" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>2023</v>
       </c>
@@ -1574,13 +1574,13 @@
         <v>17</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D73" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>2013</v>
       </c>
@@ -1588,13 +1588,13 @@
         <v>7</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D74" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>2012</v>
       </c>
@@ -1602,13 +1602,13 @@
         <v>7</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D75" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>2007</v>
       </c>
@@ -1616,13 +1616,13 @@
         <v>3</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D76" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>2006</v>
       </c>
@@ -1630,13 +1630,13 @@
         <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D77" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>2022</v>
       </c>
@@ -1644,27 +1644,27 @@
         <v>17</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D78" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>2022</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D79" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>2019</v>
       </c>
@@ -1675,10 +1675,10 @@
         <v>28</v>
       </c>
       <c r="D80" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>2014</v>
       </c>
@@ -1689,10 +1689,10 @@
         <v>28</v>
       </c>
       <c r="D81" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>2013</v>
       </c>
@@ -1703,10 +1703,10 @@
         <v>28</v>
       </c>
       <c r="D82" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>2011</v>
       </c>
@@ -1717,10 +1717,10 @@
         <v>28</v>
       </c>
       <c r="D83" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>2009</v>
       </c>
@@ -1731,10 +1731,10 @@
         <v>28</v>
       </c>
       <c r="D84" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>2006</v>
       </c>
@@ -1745,10 +1745,10 @@
         <v>28</v>
       </c>
       <c r="D85" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>2005</v>
       </c>
@@ -1759,10 +1759,10 @@
         <v>28</v>
       </c>
       <c r="D86" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>2004</v>
       </c>
@@ -1773,10 +1773,10 @@
         <v>28</v>
       </c>
       <c r="D87" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>2024</v>
       </c>
@@ -1784,13 +1784,13 @@
         <v>15</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D88" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>2024</v>
       </c>
@@ -1798,83 +1798,83 @@
         <v>18</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D89" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>2024</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D90" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>2024</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D91" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>2024</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D92" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>2024</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D93" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>2024</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>2023</v>
       </c>
@@ -1882,13 +1882,13 @@
         <v>17</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D95" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>2023</v>
       </c>
@@ -1896,27 +1896,27 @@
         <v>15</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D96" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>2023</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D97" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>2023</v>
       </c>
@@ -1924,27 +1924,27 @@
         <v>18</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D98" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>2023</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D99" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>2022</v>
       </c>
@@ -1952,13 +1952,13 @@
         <v>17</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D100" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>2022</v>
       </c>
@@ -1966,27 +1966,27 @@
         <v>18</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D101" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>2022</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D102" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>2022</v>
       </c>
@@ -1994,69 +1994,69 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D103" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>2022</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D104" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>2022</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D105" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>2022</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D106" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>2022</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D107" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>2021</v>
       </c>
@@ -2064,55 +2064,55 @@
         <v>5</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D108" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>2021</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D109" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>2021</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D110" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>2021</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D111" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>2019</v>
       </c>
@@ -2120,13 +2120,13 @@
         <v>20</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D112" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>2019</v>
       </c>
@@ -2134,13 +2134,13 @@
         <v>19</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D113" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>2019</v>
       </c>
@@ -2148,41 +2148,41 @@
         <v>5</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D114" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>2019</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D115" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>2019</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D116" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>2018</v>
       </c>
@@ -2190,13 +2190,13 @@
         <v>20</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D117" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>2018</v>
       </c>
@@ -2204,27 +2204,27 @@
         <v>19</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D118" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>2018</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D119" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>2017</v>
       </c>
@@ -2232,27 +2232,27 @@
         <v>21</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D120" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>2017</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D121" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>2017</v>
       </c>
@@ -2260,13 +2260,13 @@
         <v>20</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D122" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>2016</v>
       </c>
@@ -2274,13 +2274,13 @@
         <v>21</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D123" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>2016</v>
       </c>
@@ -2288,41 +2288,41 @@
         <v>22</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D124" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>2016</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D125" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>2016</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D126" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>2015</v>
       </c>
@@ -2330,27 +2330,27 @@
         <v>21</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D127" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>2015</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D128" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>2015</v>
       </c>
@@ -2358,13 +2358,13 @@
         <v>22</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D129" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>2014</v>
       </c>
@@ -2372,27 +2372,27 @@
         <v>23</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D130" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>2014</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D131" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>2014</v>
       </c>
@@ -2400,13 +2400,13 @@
         <v>24</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D132" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>2014</v>
       </c>
@@ -2414,27 +2414,27 @@
         <v>22</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D133" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>2014</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D134" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>2013</v>
       </c>
@@ -2442,13 +2442,13 @@
         <v>7</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D135" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>2013</v>
       </c>
@@ -2456,13 +2456,13 @@
         <v>24</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D136" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>2013</v>
       </c>
@@ -2470,27 +2470,27 @@
         <v>23</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D137" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>2013</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D138" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>2012</v>
       </c>
@@ -2498,13 +2498,13 @@
         <v>7</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D139" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>2012</v>
       </c>
@@ -2512,13 +2512,13 @@
         <v>8</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D140" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>2012</v>
       </c>
@@ -2526,13 +2526,13 @@
         <v>24</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D141" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>2011</v>
       </c>
@@ -2540,27 +2540,27 @@
         <v>7</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D142" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>2011</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D143" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>2011</v>
       </c>
@@ -2568,55 +2568,55 @@
         <v>8</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D144" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>2011</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D145" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>2011</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D146" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>2010</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D147" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>2010</v>
       </c>
@@ -2624,139 +2624,139 @@
         <v>7</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D148" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>2010</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D149" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>2009</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D150" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>2009</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D151" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>2009</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D152" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>2009</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D153" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>2008</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D154" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>2008</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D155" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>2008</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D156" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>2008</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D157" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>2007</v>
       </c>
@@ -2764,13 +2764,13 @@
         <v>3</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D158" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>2007</v>
       </c>
@@ -2778,13 +2778,13 @@
         <v>9</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D159" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>2007</v>
       </c>
@@ -2792,41 +2792,41 @@
         <v>12</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D160" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>2007</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D161" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>2007</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D162" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>2006</v>
       </c>
@@ -2834,13 +2834,13 @@
         <v>3</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D163" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>2006</v>
       </c>
@@ -2848,13 +2848,13 @@
         <v>10</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D164" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>2006</v>
       </c>
@@ -2862,13 +2862,13 @@
         <v>9</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D165" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>2006</v>
       </c>
@@ -2876,13 +2876,13 @@
         <v>11</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D166" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>2006</v>
       </c>
@@ -2890,13 +2890,13 @@
         <v>12</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D167" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>2006</v>
       </c>
@@ -2904,13 +2904,13 @@
         <v>13</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D168" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>2006</v>
       </c>
@@ -2918,13 +2918,13 @@
         <v>14</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D169" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>2006</v>
       </c>
@@ -2932,27 +2932,27 @@
         <v>26</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D170" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>2006</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D171" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>2005</v>
       </c>
@@ -2960,13 +2960,13 @@
         <v>11</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D172" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>2005</v>
       </c>
@@ -2974,13 +2974,13 @@
         <v>10</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D173" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>2005</v>
       </c>
@@ -2988,13 +2988,13 @@
         <v>26</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D174" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>2005</v>
       </c>
@@ -3002,13 +3002,13 @@
         <v>14</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D175" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>2005</v>
       </c>
@@ -3016,27 +3016,27 @@
         <v>13</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D176" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>2005</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D177" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>2004</v>
       </c>
@@ -3044,13 +3044,13 @@
         <v>3</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D178" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>2004</v>
       </c>
@@ -3058,13 +3058,13 @@
         <v>14</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D179" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>2004</v>
       </c>
@@ -3072,27 +3072,27 @@
         <v>11</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D180" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>2004</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D181" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>2004</v>
       </c>
@@ -3100,13 +3100,13 @@
         <v>13</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D182" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>2004</v>
       </c>
@@ -3114,27 +3114,27 @@
         <v>26</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D183" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>2003</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D184" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>2003</v>
       </c>
@@ -3142,24 +3142,24 @@
         <v>26</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D185" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>2003</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D186" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>